<commit_message>
Adding images and Overleaf backup
</commit_message>
<xml_diff>
--- a/Significance.xlsx
+++ b/Significance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TuDublin\Masters Project\Git Clone\MastersProject2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC6C3CA-D920-492A-B80B-162BE66F9305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0B486D-1363-47DF-80B3-ABFB9F244FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72CD5FCD-31EB-4965-8DC7-7F8A1EE5DAEE}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>